<commit_message>
Latest report and Sim
</commit_message>
<xml_diff>
--- a/Phase1/Kcalculations.xlsx
+++ b/Phase1/Kcalculations.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Alex/Documents/University/Year 4/Sensors, Signals and Control/Control/Coursework/Phase1/SSCPhase1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Alex/Documents/University/Year 4/Sensors, Signals and Control/Control/Coursework/Phase123/Phase1/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16680" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16680" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -111,7 +111,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -347,11 +347,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-259568384"/>
-        <c:axId val="-277783648"/>
+        <c:axId val="-1666793424"/>
+        <c:axId val="-1666792896"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-259568384"/>
+        <c:axId val="-1666793424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2.0"/>
@@ -470,12 +470,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-277783648"/>
+        <c:crossAx val="-1666792896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-277783648"/>
+        <c:axId val="-1666792896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -551,6 +551,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -587,7 +588,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-259568384"/>
+        <c:crossAx val="-1666793424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1496,8 +1497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:O37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G14" zoomScale="161" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1775,7 +1776,7 @@
     </row>
     <row r="18" spans="11:15" x14ac:dyDescent="0.2">
       <c r="K18">
-        <f t="shared" ref="K18:M18" si="3">$O$15*K16+$O$16</f>
+        <f t="shared" ref="K18:L18" si="3">$O$15*K16+$O$16</f>
         <v>5.4010999999999996</v>
       </c>
       <c r="L18">

</xml_diff>